<commit_message>
chore UGN-356 - add tests and update readme for new prop dateFormat
</commit_message>
<xml_diff>
--- a/static/Workbook1.xlsx
+++ b/static/Workbook1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julitakriauciunaite/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julitakriauciunaite/Desktop/Repositories/react-spreadsheet-import/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -102,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,29 +399,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>50</v>
       </c>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>